<commit_message>
Better test of setFullCalcOnLoad
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\GitHub\php-xslx-fast-editor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F694018-281E-4AD8-946F-2D10BC6206FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75814993-7380-4B93-9C1C-566FDA132B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="5580" windowWidth="24015" windowHeight="14400" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
+    <workbookView xWindow="11085" yWindow="5100" windowWidth="24015" windowHeight="14400" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Strings</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>naïveté</t>
+  </si>
+  <si>
+    <t>Formula</t>
   </si>
 </sst>
 </file>
@@ -111,7 +114,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -144,13 +150,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}" name="Tableau1" displayName="Tableau1" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}" name="Tableau1" displayName="Tableau1" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BA001A0E-7749-45F9-8C04-FDD0EAC5A690}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="0">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -161,13 +170,13 @@
   <autoFilter ref="A1:D4" xr:uid="{F3BED645-331D-480A-A4AB-D64543F12FD2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AA5B4808-251C-4118-98A6-04AAC69B263E}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{CE27FB71-EAF3-4E83-9731-8A2F1411D076}" name="Strings" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{CE27FB71-EAF3-4E83-9731-8A2F1411D076}" name="Strings" dataDxfId="3">
       <calculatedColumnFormula>Sheet1!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E6752397-B5AA-4DE4-A617-BE4D016F85F2}" name="Integers" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{E6752397-B5AA-4DE4-A617-BE4D016F85F2}" name="Integers" dataDxfId="2">
       <calculatedColumnFormula>Sheet1!C2*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C54D1C31-B322-412C-9986-0C3C251011EE}" name="Floats" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{C54D1C31-B322-412C-9986-0C3C251011EE}" name="Floats" dataDxfId="1">
       <calculatedColumnFormula>Sheet1!D2*2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -472,7 +481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB1519B-06E9-4B26-9142-D268F6CA6EED}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -484,7 +493,7 @@
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -497,8 +506,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -511,8 +523,12 @@
       <c r="D2" s="3">
         <v>3.1415899999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
+        <v>21.991129999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -525,8 +541,12 @@
       <c r="D3" s="3">
         <v>2.71828</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
+        <v>-13.5914</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -538,6 +558,10 @@
       </c>
       <c r="D4" s="3">
         <v>-1</v>
+      </c>
+      <c r="E4">
+        <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
+        <v>-128</v>
       </c>
     </row>
   </sheetData>
@@ -553,7 +577,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4CCC2D-A1AD-4627-9792-8186A023C832}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add read/write hyperlinks And some refactoring
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\GitHub\php-xslx-fast-editor\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alexandre\GitHub\php-xlsx-fast-editor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2DCD29-86CE-428E-8D0F-4A4894F8054E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C28061-F21D-4696-8ACA-14A28D534F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12135" yWindow="6150" windowWidth="24015" windowHeight="14400" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
+    <workbookView xWindow="6645" yWindow="4080" windowWidth="28800" windowHeight="15315" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,10 +82,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,17 +116,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -192,7 +203,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -492,7 +503,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -521,7 +532,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2">
@@ -557,7 +568,7 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
@@ -584,16 +595,19 @@
       <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{E9E8ECA9-6693-4D6C-ADAA-05FA71C5DE84}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -602,11 +616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4CCC2D-A1AD-4627-9792-8186A023C832}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Add support for reading dates
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alexandre\GitHub\php-xlsx-fast-editor\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\GitHub\php-xslx-fast-editor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C28061-F21D-4696-8ACA-14A28D534F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6390C5F-1FEB-41FC-8468-C8E8742319A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="4080" windowWidth="28800" windowHeight="15315" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
+    <workbookView xWindow="10980" yWindow="6210" windowWidth="24015" windowHeight="14400" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Strings</t>
   </si>
@@ -76,12 +76,20 @@
   </si>
   <si>
     <t>Four</t>
+  </si>
+  <si>
+    <t>DateTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,19 +128,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -141,6 +151,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -168,16 +181,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}" name="Tableau1" displayName="Tableau1" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}" name="Tableau1" displayName="Tableau1" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BA001A0E-7749-45F9-8C04-FDD0EAC5A690}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="4">
       <calculatedColumnFormula>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -203,7 +217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,19 +513,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB1519B-06E9-4B26-9142-D268F6CA6EED}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -527,12 +544,15 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2">
@@ -545,8 +565,11 @@
         <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
         <v>21.991129999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="5">
+        <v>29549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -563,12 +586,15 @@
         <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
         <v>-13.5914</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="6">
+        <v>29549.430902777778</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
@@ -581,8 +607,11 @@
         <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
         <v>-128</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="7">
+        <v>0.4309027777777778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -598,6 +627,9 @@
       <c r="E5">
         <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
         <v>12</v>
+      </c>
+      <c r="F5" s="6">
+        <v>29549.430902777778</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +650,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Support formatted shared strings Make the `->readString()` function more robust and work also with strings containing several formattings
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\GitHub\php-xslx-fast-editor\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alexandre\GitHub\php-xlsx-fast-editor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6390C5F-1FEB-41FC-8468-C8E8742319A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B730E6-1433-44F1-8C50-7845671AEB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10980" yWindow="6210" windowWidth="24015" windowHeight="14400" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Example 3</t>
   </si>
   <si>
-    <t>déjà-vu</t>
-  </si>
-  <si>
     <t>naïveté</t>
   </si>
   <si>
@@ -79,6 +76,40 @@
   </si>
   <si>
     <t>DateTime</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>déjà</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>vu</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -90,7 +121,7 @@
     <numFmt numFmtId="165" formatCode="d/m/yy\ h:mm;@"/>
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +136,29 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,7 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -137,9 +191,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -217,7 +272,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -515,20 +570,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB1519B-06E9-4B26-9142-D268F6CA6EED}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -542,13 +595,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -569,12 +622,12 @@
         <v>29549</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="2">
         <v>-5</v>
@@ -590,12 +643,12 @@
         <v>29549.430902777778</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>128</v>
@@ -611,12 +664,12 @@
         <v>0.4309027777777778</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -650,15 +703,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -672,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -689,7 +742,7 @@
         <v>6.2831799999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -706,7 +759,7 @@
         <v>5.4365600000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Fix sheet reference fix https://github.com/alexandrainst/php-xlsx-fast-editor/issues/15 Fix `XlsxFastEditor::getWorksheetNumber()` which was not returning the proper number in case of workbooks in which sheets have been reordered or removed.
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alexandre\GitHub\php-xlsx-fast-editor\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\GitHub\php-xslx-fast-editor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A3BE05-968A-419E-8F46-EBE0813908FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8CADEA-DC05-4B5D-9650-2D54AB145FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="4140" windowWidth="28800" windowHeight="15435" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
+    <workbookView xWindow="5685" yWindow="1125" windowWidth="29235" windowHeight="18750" activeTab="2" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -198,7 +198,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -240,23 +240,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}" name="Tableau1" displayName="Tableau1" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BA001A0E-7749-45F9-8C04-FDD0EAC5A690}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="4">
-      <calculatedColumnFormula>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3BED645-331D-480A-A4AB-D64543F12FD2}" name="Tableau13" displayName="Tableau13" ref="A1:D4" totalsRowShown="0">
   <autoFilter ref="A1:D4" xr:uid="{F3BED645-331D-480A-A4AB-D64543F12FD2}"/>
   <tableColumns count="4">
@@ -275,10 +258,27 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}" name="Tableau1" displayName="Tableau1" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{BA001A0E-7749-45F9-8C04-FDD0EAC5A690}" name="Examples"/>
+    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="4">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,7 +316,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -422,7 +422,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -564,19 +564,201 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4CCC2D-A1AD-4627-9792-8186A023C832}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>Sheet1!B2</f>
+        <v>Hello</v>
+      </c>
+      <c r="C2" s="2">
+        <f>Sheet1!C2*2</f>
+        <v>14</v>
+      </c>
+      <c r="D2" s="3">
+        <f>Sheet1!D2*2</f>
+        <v>6.2831799999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>Sheet1!B3</f>
+        <v>déjà-vu</v>
+      </c>
+      <c r="C3" s="2">
+        <f>Sheet1!C3*2</f>
+        <v>-10</v>
+      </c>
+      <c r="D3" s="3">
+        <f>Sheet1!D3*2</f>
+        <v>5.4365600000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>Sheet1!B4</f>
+        <v>naïveté</v>
+      </c>
+      <c r="C4" s="2">
+        <f>Sheet1!C4*2</f>
+        <v>256</v>
+      </c>
+      <c r="D4" s="3">
+        <f>Sheet1!D4*2</f>
+        <v>-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED8FD1B-ED9A-4555-AB46-56C88316F5F7}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB1519B-06E9-4B26-9142-D268F6CA6EED}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -699,186 +881,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4CCC2D-A1AD-4627-9792-8186A023C832}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <f>Sheet1!B2</f>
-        <v>Hello</v>
-      </c>
-      <c r="C2" s="2">
-        <f>Sheet1!C2*2</f>
-        <v>14</v>
-      </c>
-      <c r="D2" s="3">
-        <f>Sheet1!D2*2</f>
-        <v>6.2831799999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="str">
-        <f>Sheet1!B3</f>
-        <v>déjà-vu</v>
-      </c>
-      <c r="C3" s="2">
-        <f>Sheet1!C3*2</f>
-        <v>-10</v>
-      </c>
-      <c r="D3" s="3">
-        <f>Sheet1!D3*2</f>
-        <v>5.4365600000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f>Sheet1!B4</f>
-        <v>naïveté</v>
-      </c>
-      <c r="C4" s="2">
-        <f>Sheet1!C4*2</f>
-        <v>256</v>
-      </c>
-      <c r="D4" s="3">
-        <f>Sheet1!D4*2</f>
-        <v>-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED8FD1B-ED9A-4555-AB46-56C88316F5F7}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix sheet reference (#16)
fix https://github.com/alexandrainst/php-xlsx-fast-editor/issues/15
Fix `XlsxFastEditor::getWorksheetNumber()` which was not returning the proper number in case of workbooks in which sheets have been reordered or removed.
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alexandre\GitHub\php-xlsx-fast-editor\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\GitHub\php-xslx-fast-editor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A3BE05-968A-419E-8F46-EBE0813908FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8CADEA-DC05-4B5D-9650-2D54AB145FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="4140" windowWidth="28800" windowHeight="15435" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
+    <workbookView xWindow="5685" yWindow="1125" windowWidth="29235" windowHeight="18750" activeTab="2" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -198,7 +198,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -240,23 +240,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}" name="Tableau1" displayName="Tableau1" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BA001A0E-7749-45F9-8C04-FDD0EAC5A690}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="4">
-      <calculatedColumnFormula>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F3BED645-331D-480A-A4AB-D64543F12FD2}" name="Tableau13" displayName="Tableau13" ref="A1:D4" totalsRowShown="0">
   <autoFilter ref="A1:D4" xr:uid="{F3BED645-331D-480A-A4AB-D64543F12FD2}"/>
   <tableColumns count="4">
@@ -275,10 +258,27 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}" name="Tableau1" displayName="Tableau1" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{BA001A0E-7749-45F9-8C04-FDD0EAC5A690}" name="Examples"/>
+    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="4">
+      <calculatedColumnFormula>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,7 +316,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -422,7 +422,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -564,19 +564,201 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4CCC2D-A1AD-4627-9792-8186A023C832}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>Sheet1!B2</f>
+        <v>Hello</v>
+      </c>
+      <c r="C2" s="2">
+        <f>Sheet1!C2*2</f>
+        <v>14</v>
+      </c>
+      <c r="D2" s="3">
+        <f>Sheet1!D2*2</f>
+        <v>6.2831799999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>Sheet1!B3</f>
+        <v>déjà-vu</v>
+      </c>
+      <c r="C3" s="2">
+        <f>Sheet1!C3*2</f>
+        <v>-10</v>
+      </c>
+      <c r="D3" s="3">
+        <f>Sheet1!D3*2</f>
+        <v>5.4365600000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>Sheet1!B4</f>
+        <v>naïveté</v>
+      </c>
+      <c r="C4" s="2">
+        <f>Sheet1!C4*2</f>
+        <v>256</v>
+      </c>
+      <c r="D4" s="3">
+        <f>Sheet1!D4*2</f>
+        <v>-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED8FD1B-ED9A-4555-AB46-56C88316F5F7}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB1519B-06E9-4B26-9142-D268F6CA6EED}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -699,186 +881,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4CCC2D-A1AD-4627-9792-8186A023C832}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <f>Sheet1!B2</f>
-        <v>Hello</v>
-      </c>
-      <c r="C2" s="2">
-        <f>Sheet1!C2*2</f>
-        <v>14</v>
-      </c>
-      <c r="D2" s="3">
-        <f>Sheet1!D2*2</f>
-        <v>6.2831799999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="str">
-        <f>Sheet1!B3</f>
-        <v>déjà-vu</v>
-      </c>
-      <c r="C3" s="2">
-        <f>Sheet1!C3*2</f>
-        <v>-10</v>
-      </c>
-      <c r="D3" s="3">
-        <f>Sheet1!D3*2</f>
-        <v>5.4365600000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f>Sheet1!B4</f>
-        <v>naïveté</v>
-      </c>
-      <c r="C4" s="2">
-        <f>Sheet1!C4*2</f>
-        <v>256</v>
-      </c>
-      <c r="D4" s="3">
-        <f>Sheet1!D4*2</f>
-        <v>-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED8FD1B-ED9A-4555-AB46-56C88316F5F7}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Improve floating point precision logic
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\GitHub\php-xslx-fast-editor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8CADEA-DC05-4B5D-9650-2D54AB145FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2A2B55-3562-49B5-BD20-DE77D64D8F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="1125" windowWidth="29235" windowHeight="18750" activeTab="2" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
+    <workbookView xWindow="7380" yWindow="5820" windowWidth="25830" windowHeight="15090" activeTab="2" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -120,10 +120,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="d/m/yy\ h:mm;@"/>
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -186,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -196,21 +197,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
@@ -225,6 +218,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -244,13 +246,13 @@
   <autoFilter ref="A1:D4" xr:uid="{F3BED645-331D-480A-A4AB-D64543F12FD2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AA5B4808-251C-4118-98A6-04AAC69B263E}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{CE27FB71-EAF3-4E83-9731-8A2F1411D076}" name="Strings" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{CE27FB71-EAF3-4E83-9731-8A2F1411D076}" name="Strings" dataDxfId="7">
       <calculatedColumnFormula>Sheet1!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E6752397-B5AA-4DE4-A617-BE4D016F85F2}" name="Integers" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{E6752397-B5AA-4DE4-A617-BE4D016F85F2}" name="Integers" dataDxfId="6">
       <calculatedColumnFormula>Sheet1!C2*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C54D1C31-B322-412C-9986-0C3C251011EE}" name="Floats" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{C54D1C31-B322-412C-9986-0C3C251011EE}" name="Floats" dataDxfId="5">
       <calculatedColumnFormula>Sheet1!D2*2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -263,13 +265,13 @@
   <autoFilter ref="A1:F5" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BA001A0E-7749-45F9-8C04-FDD0EAC5A690}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="1">
       <calculatedColumnFormula>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -651,6 +653,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Aptos"&amp;10&amp;K000000 INTERNAL&amp;1#_x000D_</oddHeader>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -749,6 +754,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Aptos"&amp;10&amp;K000000 INTERNAL&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -764,7 +772,7 @@
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -825,8 +833,8 @@
         <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
         <v>-13.5914</v>
       </c>
-      <c r="F3" s="6">
-        <v>29549.430902777778</v>
+      <c r="F3" s="9">
+        <v>29549.430908055554</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -877,6 +885,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Aptos"&amp;10&amp;K000000 INTERNAL&amp;1#_x000D_</oddHeader>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>

</xml_diff>

<commit_message>
New function writeDateTime() (#45)
* Bump PHPStan

* New function writeDateTime()

* Improve floating point precision logic

* Readme date
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\GitHub\php-xslx-fast-editor\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8CADEA-DC05-4B5D-9650-2D54AB145FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2A2B55-3562-49B5-BD20-DE77D64D8F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="1125" windowWidth="29235" windowHeight="18750" activeTab="2" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
+    <workbookView xWindow="7380" yWindow="5820" windowWidth="25830" windowHeight="15090" activeTab="2" xr2:uid="{F59855BD-93E1-430D-BF37-01D8D7A45BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -120,10 +120,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="d/m/yy\ h:mm;@"/>
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -186,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -196,21 +197,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
@@ -225,6 +218,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -244,13 +246,13 @@
   <autoFilter ref="A1:D4" xr:uid="{F3BED645-331D-480A-A4AB-D64543F12FD2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AA5B4808-251C-4118-98A6-04AAC69B263E}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{CE27FB71-EAF3-4E83-9731-8A2F1411D076}" name="Strings" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{CE27FB71-EAF3-4E83-9731-8A2F1411D076}" name="Strings" dataDxfId="7">
       <calculatedColumnFormula>Sheet1!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E6752397-B5AA-4DE4-A617-BE4D016F85F2}" name="Integers" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{E6752397-B5AA-4DE4-A617-BE4D016F85F2}" name="Integers" dataDxfId="6">
       <calculatedColumnFormula>Sheet1!C2*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C54D1C31-B322-412C-9986-0C3C251011EE}" name="Floats" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{C54D1C31-B322-412C-9986-0C3C251011EE}" name="Floats" dataDxfId="5">
       <calculatedColumnFormula>Sheet1!D2*2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -263,13 +265,13 @@
   <autoFilter ref="A1:F5" xr:uid="{300BA0E6-368B-4C82-8519-9A61D74806CC}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{BA001A0E-7749-45F9-8C04-FDD0EAC5A690}" name="Examples"/>
-    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{E62B16BD-E79E-4165-8A8F-EC6E8B5BC1E9}" name="Strings" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{753964EA-2F92-4D1D-8DCE-2320D1083466}" name="Integers" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2C755EA6-52BE-45F2-A9EC-04A98880C540}" name="Floats" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{54F9A385-188B-4D83-8BA4-07516B1EB011}" name="Formula" dataDxfId="1">
       <calculatedColumnFormula>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C158B9C1-55E0-47CB-B153-86BF8A3EA2A7}" name="DateTime" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -651,6 +653,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Aptos"&amp;10&amp;K000000 INTERNAL&amp;1#_x000D_</oddHeader>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -749,6 +754,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Aptos"&amp;10&amp;K000000 INTERNAL&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -764,7 +772,7 @@
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -825,8 +833,8 @@
         <f>Tableau1[[#This Row],[Integers]]*Tableau1[[#This Row],[Floats]]</f>
         <v>-13.5914</v>
       </c>
-      <c r="F3" s="6">
-        <v>29549.430902777778</v>
+      <c r="F3" s="9">
+        <v>29549.430908055554</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -877,6 +885,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Aptos"&amp;10&amp;K000000 INTERNAL&amp;1#_x000D_</oddHeader>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>

</xml_diff>